<commit_message>
Adding Kafka queue for scheduled tasks
</commit_message>
<xml_diff>
--- a/energydeskapi/examples/flexprovider/assets_sample.xlsx
+++ b/energydeskapi/examples/flexprovider/assets_sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steinar/PycharmProjects/energydesk-python-sdk/energydeskapi/examples/flexprovider/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654AFC28-39E5-8D48-958E-5F6EAAFE66BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE5EA1B-4DAB-A44A-9A17-74B750C07A8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17940" xr2:uid="{1404326B-8303-41D0-A255-B0C49EE0FC1A}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17800" xr2:uid="{1404326B-8303-41D0-A255-B0C49EE0FC1A}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -44,12 +44,6 @@
     <t>Storkunde A</t>
   </si>
   <si>
-    <t>Elkjele A</t>
-  </si>
-  <si>
-    <t>Elkjele B</t>
-  </si>
-  <si>
     <t>Assetveien 1</t>
   </si>
   <si>
@@ -71,9 +65,6 @@
     <t>Assetskogen 12</t>
   </si>
   <si>
-    <t>Elkjele C</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -95,13 +86,22 @@
     <t>Must be legal Brønnøysundnumber</t>
   </si>
   <si>
-    <t>707057500056455200</t>
-  </si>
-  <si>
-    <t>707057500056255000</t>
-  </si>
-  <si>
-    <t>707057500057530000</t>
+    <t>Elkjele e</t>
+  </si>
+  <si>
+    <t>Elkjele f</t>
+  </si>
+  <si>
+    <t>Elkjele g</t>
+  </si>
+  <si>
+    <t>707057500051530000</t>
+  </si>
+  <si>
+    <t>707057500053255000</t>
+  </si>
+  <si>
+    <t>707057500056855200</t>
   </si>
 </sst>
 </file>
@@ -491,8 +491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AE6D704-99A5-44D7-AD78-B635010F156D}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="258" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -508,45 +508,45 @@
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="F1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F2">
         <v>10.7781987267395</v>
@@ -555,21 +555,21 @@
         <v>59.734255470387502</v>
       </c>
       <c r="H2">
-        <v>12121212</v>
+        <v>926956191</v>
       </c>
       <c r="I2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
         <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
@@ -584,24 +584,24 @@
         <v>59.634255470387501</v>
       </c>
       <c r="H3">
-        <v>12121212</v>
+        <v>918874321</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F4">
         <v>10.678198726739501</v>
@@ -610,7 +610,7 @@
         <v>59.5342554703875</v>
       </c>
       <c r="H4">
-        <v>12121212</v>
+        <v>913303334</v>
       </c>
     </row>
   </sheetData>
@@ -624,6 +624,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7cca4d28-be15-4989-9e30-9ac6a8d8433a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="8f85b5cd-6a4f-4481-9dd1-a01af0963407" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100DE8F542BB1CD124680DA011DB3AEBBA3" ma:contentTypeVersion="13" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="8dd1152b8817e425c021184c0baf5a3a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7cca4d28-be15-4989-9e30-9ac6a8d8433a" xmlns:ns3="8f85b5cd-6a4f-4481-9dd1-a01af0963407" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7c0a5638ef26eedfe013bdba548b26e7" ns2:_="" ns3:_="">
     <xsd:import namespace="7cca4d28-be15-4989-9e30-9ac6a8d8433a"/>
@@ -846,27 +866,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E073A28F-5DF8-4A81-ABA4-2B60C2E73862}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="8f85b5cd-6a4f-4481-9dd1-a01af0963407"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="7cca4d28-be15-4989-9e30-9ac6a8d8433a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7cca4d28-be15-4989-9e30-9ac6a8d8433a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="8f85b5cd-6a4f-4481-9dd1-a01af0963407" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{293C9471-FADF-4AF4-AC67-33A988CCF802}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBD2B694-A2B4-4F2A-AFAD-B7A3012793F2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -883,29 +908,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{293C9471-FADF-4AF4-AC67-33A988CCF802}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E073A28F-5DF8-4A81-ABA4-2B60C2E73862}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="8f85b5cd-6a4f-4481-9dd1-a01af0963407"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="7cca4d28-be15-4989-9e30-9ac6a8d8433a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>